<commit_message>
Pushed to github now
</commit_message>
<xml_diff>
--- a/Degree.xlsx
+++ b/Degree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\AP Tamrin 3 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A65CF0-7F1C-4E20-855D-17BF2B92C995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02A6059-6DB0-4928-8C58-CDB715AC320D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A019F027-8123-4CDF-BE62-E60F7E5B0D6F}"/>
   </bookViews>
@@ -1060,7 +1060,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
just wensday have empty time
</commit_message>
<xml_diff>
--- a/Degree.xlsx
+++ b/Degree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\AP Tamrin 3 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AE25BC-CEDD-461E-A8F3-2BCE087258F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88D8138-8F55-4BFD-ABDC-FEB377D9A915}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A019F027-8123-4CDF-BE62-E60F7E5B0D6F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -151,6 +151,18 @@
   </si>
   <si>
     <t>محسن سعیدآبادی</t>
+  </si>
+  <si>
+    <t>ali soltani</t>
+  </si>
+  <si>
+    <t>soltanibookali1380@gmail.com</t>
+  </si>
+  <si>
+    <t>Arman Sinaei</t>
+  </si>
+  <si>
+    <t>armansinaie1380@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -646,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -744,6 +756,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1081,7 +1096,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1096,16 +1111,16 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="34.799999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="36" t="s">
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="36"/>
+      <c r="K2" s="37"/>
     </row>
     <row r="3" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
@@ -1163,7 +1178,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
-      <c r="L4" s="37" t="s">
+      <c r="L4" s="38" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1189,7 +1204,7 @@
       <c r="I5" s="10"/>
       <c r="J5" s="16"/>
       <c r="K5" s="17"/>
-      <c r="L5" s="37"/>
+      <c r="L5" s="38"/>
     </row>
     <row r="6" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
@@ -1213,15 +1228,21 @@
       <c r="I6" s="10"/>
       <c r="J6" s="16"/>
       <c r="K6" s="17"/>
-      <c r="L6" s="37"/>
+      <c r="L6" s="38"/>
     </row>
     <row r="7" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="23"/>
+      <c r="A7" s="23" t="s">
+        <v>41</v>
+      </c>
       <c r="B7" s="19">
         <v>4</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
+      <c r="C7" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="35">
+        <v>99521343</v>
+      </c>
       <c r="E7" s="19" t="s">
         <v>15</v>
       </c>
@@ -1231,7 +1252,7 @@
       <c r="I7" s="13"/>
       <c r="J7" s="27"/>
       <c r="K7" s="28"/>
-      <c r="L7" s="37"/>
+      <c r="L7" s="38"/>
     </row>
     <row r="8" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="21" t="s">
@@ -1255,17 +1276,23 @@
       <c r="I8" s="7"/>
       <c r="J8" s="25"/>
       <c r="K8" s="26"/>
-      <c r="L8" s="38" t="s">
+      <c r="L8" s="39" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="23"/>
+      <c r="A9" s="23" t="s">
+        <v>43</v>
+      </c>
       <c r="B9" s="19">
         <v>6</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="C9" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="35">
+        <v>99521352</v>
+      </c>
       <c r="E9" s="19" t="s">
         <v>17</v>
       </c>
@@ -1275,7 +1302,7 @@
       <c r="I9" s="13"/>
       <c r="J9" s="27"/>
       <c r="K9" s="28"/>
-      <c r="L9" s="39"/>
+      <c r="L9" s="40"/>
     </row>
     <row r="10" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="21" t="s">
@@ -1299,7 +1326,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="25"/>
       <c r="K10" s="26"/>
-      <c r="L10" s="38" t="s">
+      <c r="L10" s="39" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1319,7 +1346,7 @@
       <c r="I11" s="10"/>
       <c r="J11" s="16"/>
       <c r="K11" s="17"/>
-      <c r="L11" s="40"/>
+      <c r="L11" s="41"/>
     </row>
     <row r="12" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="22"/>
@@ -1337,7 +1364,7 @@
       <c r="I12" s="10"/>
       <c r="J12" s="16"/>
       <c r="K12" s="17"/>
-      <c r="L12" s="40"/>
+      <c r="L12" s="41"/>
     </row>
     <row r="13" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="22"/>
@@ -1355,7 +1382,7 @@
       <c r="I13" s="10"/>
       <c r="J13" s="16"/>
       <c r="K13" s="17"/>
-      <c r="L13" s="40"/>
+      <c r="L13" s="41"/>
     </row>
     <row r="14" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="23" t="s">
@@ -1379,7 +1406,7 @@
       <c r="I14" s="13"/>
       <c r="J14" s="27"/>
       <c r="K14" s="28"/>
-      <c r="L14" s="39"/>
+      <c r="L14" s="40"/>
     </row>
     <row r="15" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="29" t="s">

</xml_diff>

<commit_message>
Update sheet and add delay percentage
</commit_message>
<xml_diff>
--- a/Degree.xlsx
+++ b/Degree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\AP Tamrin 3 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468A811B-E64A-4F8E-943B-9A18003F9CB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740EC9A6-23C8-427B-8AAE-D073178587AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A019F027-8123-4CDF-BE62-E60F7E5B0D6F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -69,18 +69,12 @@
     <t>danialzenoozi79@gmail.com</t>
   </si>
   <si>
-    <t>27  1:00</t>
-  </si>
-  <si>
     <t>27  1:45</t>
   </si>
   <si>
     <t>27  2:30</t>
   </si>
   <si>
-    <t>27  3:15</t>
-  </si>
-  <si>
     <t>28  3:30</t>
   </si>
   <si>
@@ -165,7 +159,22 @@
     <t>armansinaie1380@gmail.com</t>
   </si>
   <si>
-    <t>*</t>
+    <t>مجتبی صفری محمد آبادی</t>
+  </si>
+  <si>
+    <t>112.5 90per</t>
+  </si>
+  <si>
+    <t>88 90per</t>
+  </si>
+  <si>
+    <t>90 90per</t>
+  </si>
+  <si>
+    <t>70per</t>
+  </si>
+  <si>
+    <t>90per</t>
   </si>
 </sst>
 </file>
@@ -211,7 +220,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,12 +251,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="31">
     <border>
@@ -673,7 +676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -782,25 +785,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -819,6 +804,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -1135,10 +1123,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54BD848E-E297-4097-8BEE-9ABC561FDC7A}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.8" x14ac:dyDescent="0.3"/>
@@ -1153,20 +1141,20 @@
     <col min="14" max="18" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="23.4" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:13" ht="34.799999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F2" s="45" t="s">
+    <row r="1" spans="1:12" ht="23.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:12" ht="34.799999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="46" t="s">
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="46"/>
-    </row>
-    <row r="3" spans="1:13" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K2" s="40"/>
+    </row>
+    <row r="3" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1200,345 +1188,349 @@
       </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:13" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="39">
+    <row r="4" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="39">
-        <v>99521298</v>
-      </c>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="8">
+        <v>99300066</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" s="37" t="s">
+      <c r="F4" s="22" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="8">
+      <c r="G4" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="25">
+        <v>80</v>
+      </c>
+      <c r="K4" s="26">
+        <v>80</v>
+      </c>
+      <c r="L4" s="41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="38">
         <v>2</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D5" s="8">
-        <v>99300066</v>
+        <v>98441279</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="22">
-        <v>60</v>
+      <c r="F5" s="22" t="s">
+        <v>43</v>
       </c>
       <c r="G5" s="23">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H5" s="23">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="I5" s="24">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="J5" s="25">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="K5" s="26">
-        <v>70</v>
-      </c>
-      <c r="L5" s="47"/>
-    </row>
-    <row r="6" spans="1:13" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="8">
+        <v>100</v>
+      </c>
+      <c r="L5" s="41"/>
+    </row>
+    <row r="6" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="38">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="8">
-        <v>98441279</v>
+      <c r="C6" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="13">
+        <v>99521316</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="22">
-        <v>125</v>
-      </c>
-      <c r="G6" s="23">
+      <c r="F6" s="18">
+        <v>120</v>
+      </c>
+      <c r="G6" s="19">
         <v>100</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="19">
         <v>100</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I6" s="17">
         <v>100</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="20">
         <v>100</v>
       </c>
-      <c r="K6" s="26">
-        <v>90</v>
-      </c>
-      <c r="L6" s="47"/>
-    </row>
-    <row r="7" spans="1:13" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K6" s="21">
+        <v>100</v>
+      </c>
+      <c r="L6" s="42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="38">
         <v>4</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="15">
-        <v>99521343</v>
+        <v>99521352</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="37" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F7" s="27">
+        <v>125</v>
+      </c>
+      <c r="G7" s="28">
+        <v>100</v>
+      </c>
+      <c r="H7" s="28">
+        <v>100</v>
+      </c>
+      <c r="I7" s="29">
+        <v>100</v>
+      </c>
+      <c r="J7" s="30">
+        <v>100</v>
+      </c>
+      <c r="K7" s="31">
+        <v>100</v>
+      </c>
+      <c r="L7" s="43"/>
+    </row>
+    <row r="8" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="8">
+        <v>23</v>
+      </c>
+      <c r="B8" s="38">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="13">
-        <v>99521316</v>
+      <c r="C8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="8">
+        <v>99521262</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="18">
-        <v>120</v>
-      </c>
-      <c r="G8" s="19">
-        <v>100</v>
-      </c>
-      <c r="H8" s="19">
-        <v>100</v>
-      </c>
-      <c r="I8" s="17">
-        <v>100</v>
-      </c>
-      <c r="J8" s="20">
-        <v>100</v>
-      </c>
-      <c r="K8" s="21">
-        <v>90</v>
-      </c>
-      <c r="L8" s="48" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="8">
+        <v>21</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
+      <c r="B9" s="38">
         <v>6</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="15">
-        <v>99521352</v>
-      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="49"/>
-    </row>
-    <row r="10" spans="1:13" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="8">
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="44"/>
+    </row>
+    <row r="10" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="38">
         <v>7</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="8">
-        <v>99521262</v>
+      <c r="C10" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="38">
+        <v>99521343</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="48" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="11"/>
-      <c r="B11" s="8">
+        <v>18</v>
+      </c>
+      <c r="F10" s="22">
+        <v>0</v>
+      </c>
+      <c r="G10" s="23">
+        <v>0</v>
+      </c>
+      <c r="H10" s="23">
+        <v>0</v>
+      </c>
+      <c r="I10" s="24">
+        <v>0</v>
+      </c>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="44"/>
+    </row>
+    <row r="11" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="38">
         <v>8</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="C11" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="8">
+        <v>99521298</v>
+      </c>
       <c r="E11" s="8" t="s">
         <v>19</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
-      <c r="I11" s="24"/>
+      <c r="I11" s="24">
+        <v>100</v>
+      </c>
       <c r="J11" s="25"/>
       <c r="K11" s="26"/>
-      <c r="L11" s="50"/>
-    </row>
-    <row r="12" spans="1:13" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="11"/>
-      <c r="B12" s="8">
+      <c r="L11" s="44"/>
+    </row>
+    <row r="12" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="38">
         <v>9</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="8">
+        <v>97411477</v>
+      </c>
       <c r="E12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="50"/>
-    </row>
-    <row r="13" spans="1:13" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="8">
+      <c r="F12" s="27"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="43"/>
+    </row>
+    <row r="13" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="38">
         <v>10</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="8">
-        <v>99521298</v>
+      <c r="C13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="13">
+        <v>99300093</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="24">
-        <v>100</v>
-      </c>
-      <c r="J13" s="25"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="50"/>
-    </row>
-    <row r="14" spans="1:13" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="8">
-        <v>11</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="8">
-        <v>97411477</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="49"/>
-    </row>
-    <row r="15" spans="1:13" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="8">
-        <v>12</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="13">
-        <v>99300093</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="23.4" thickTop="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="K13" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="23.4" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="2"/>
+      <c r="C15" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
@@ -1619,39 +1611,13 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L4:L7"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="L10:L14"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="L8:L12"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mohammad darmanloo degree added
</commit_message>
<xml_diff>
--- a/Degree.xlsx
+++ b/Degree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\AP Tamrin 3 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740EC9A6-23C8-427B-8AAE-D073178587AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875FC580-8B89-4880-A497-FC9B0AA2FD34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A019F027-8123-4CDF-BE62-E60F7E5B0D6F}"/>
   </bookViews>
@@ -788,6 +788,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -804,9 +807,6 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -1126,7 +1126,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.8" x14ac:dyDescent="0.3"/>
@@ -1143,16 +1143,16 @@
   <sheetData>
     <row r="1" spans="1:12" ht="23.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="34.799999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40" t="s">
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="40"/>
+      <c r="K2" s="41"/>
     </row>
     <row r="3" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
@@ -1222,7 +1222,7 @@
       <c r="K4" s="26">
         <v>80</v>
       </c>
-      <c r="L4" s="41" t="s">
+      <c r="L4" s="42" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1260,7 +1260,7 @@
       <c r="K5" s="26">
         <v>100</v>
       </c>
-      <c r="L5" s="41"/>
+      <c r="L5" s="42"/>
     </row>
     <row r="6" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
@@ -1296,7 +1296,7 @@
       <c r="K6" s="21">
         <v>100</v>
       </c>
-      <c r="L6" s="42" t="s">
+      <c r="L6" s="43" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1334,7 +1334,7 @@
       <c r="K7" s="31">
         <v>100</v>
       </c>
-      <c r="L7" s="43"/>
+      <c r="L7" s="44"/>
     </row>
     <row r="8" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
@@ -1352,13 +1352,25 @@
       <c r="E8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="42" t="s">
+      <c r="F8" s="18">
+        <v>125</v>
+      </c>
+      <c r="G8" s="19">
+        <v>97</v>
+      </c>
+      <c r="H8" s="19">
+        <v>92</v>
+      </c>
+      <c r="I8" s="17">
+        <v>90</v>
+      </c>
+      <c r="J8" s="20">
+        <v>105</v>
+      </c>
+      <c r="K8" s="21">
+        <v>100</v>
+      </c>
+      <c r="L8" s="43" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1378,7 +1390,7 @@
       <c r="I9" s="24"/>
       <c r="J9" s="25"/>
       <c r="K9" s="26"/>
-      <c r="L9" s="44"/>
+      <c r="L9" s="45"/>
     </row>
     <row r="10" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
@@ -1410,7 +1422,7 @@
       </c>
       <c r="J10" s="25"/>
       <c r="K10" s="26"/>
-      <c r="L10" s="44"/>
+      <c r="L10" s="45"/>
     </row>
     <row r="11" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
@@ -1436,7 +1448,7 @@
       </c>
       <c r="J11" s="25"/>
       <c r="K11" s="26"/>
-      <c r="L11" s="44"/>
+      <c r="L11" s="45"/>
     </row>
     <row r="12" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
@@ -1460,7 +1472,7 @@
       <c r="I12" s="29"/>
       <c r="J12" s="30"/>
       <c r="K12" s="31"/>
-      <c r="L12" s="43"/>
+      <c r="L12" s="44"/>
     </row>
     <row r="13" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
@@ -1507,7 +1519,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="39" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="2"/>

</xml_diff>

<commit_message>
ali soltali degree added
</commit_message>
<xml_diff>
--- a/Degree.xlsx
+++ b/Degree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\AP Tamrin 3 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875FC580-8B89-4880-A497-FC9B0AA2FD34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4C88F5-D35C-4ACB-A9C8-E1AD27C19453}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A019F027-8123-4CDF-BE62-E60F7E5B0D6F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -175,13 +175,16 @@
   </si>
   <si>
     <t>90per</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mokhtalet100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +222,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -676,7 +685,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -807,6 +816,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -1123,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54BD848E-E297-4097-8BEE-9ABC561FDC7A}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.8" x14ac:dyDescent="0.3"/>
@@ -1138,11 +1150,12 @@
     <col min="5" max="5" width="17.5546875" customWidth="1"/>
     <col min="6" max="12" width="12.88671875" customWidth="1"/>
     <col min="13" max="13" width="5.33203125" style="37" customWidth="1"/>
-    <col min="14" max="18" width="12.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" customWidth="1"/>
+    <col min="15" max="18" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="23.4" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:12" ht="34.799999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="23.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:14" ht="34.799999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F2" s="40" t="s">
         <v>9</v>
       </c>
@@ -1154,7 +1167,7 @@
       </c>
       <c r="K2" s="41"/>
     </row>
-    <row r="3" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1188,7 +1201,7 @@
       </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
@@ -1226,7 +1239,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>25</v>
       </c>
@@ -1262,7 +1275,7 @@
       </c>
       <c r="L5" s="42"/>
     </row>
-    <row r="6" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>35</v>
       </c>
@@ -1300,7 +1313,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>41</v>
       </c>
@@ -1336,7 +1349,7 @@
       </c>
       <c r="L7" s="44"/>
     </row>
-    <row r="8" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>23</v>
       </c>
@@ -1374,7 +1387,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
       <c r="B9" s="38">
         <v>6</v>
@@ -1392,7 +1405,7 @@
       <c r="K9" s="26"/>
       <c r="L9" s="45"/>
     </row>
-    <row r="10" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>39</v>
       </c>
@@ -1420,11 +1433,18 @@
       <c r="I10" s="24">
         <v>0</v>
       </c>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26"/>
+      <c r="J10" s="25">
+        <v>88</v>
+      </c>
+      <c r="K10" s="26">
+        <v>90</v>
+      </c>
       <c r="L10" s="45"/>
-    </row>
-    <row r="11" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N10" s="46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>33</v>
       </c>
@@ -1450,7 +1470,7 @@
       <c r="K11" s="26"/>
       <c r="L11" s="45"/>
     </row>
-    <row r="12" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>31</v>
       </c>
@@ -1474,7 +1494,7 @@
       <c r="K12" s="31"/>
       <c r="L12" s="44"/>
     </row>
-    <row r="13" spans="1:12" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>36</v>
       </c>
@@ -1504,7 +1524,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="23.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="23.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="1"/>
@@ -1517,7 +1537,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="39" t="s">
         <v>42</v>
@@ -1532,7 +1552,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>

</xml_diff>

<commit_message>
Submit degree in google doc
</commit_message>
<xml_diff>
--- a/Degree.xlsx
+++ b/Degree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\AP Tamrin 3 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509D14C5-4B08-414E-BB7B-2FC94FAA65C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0127A0C8-8EAC-4B1D-8AC6-BF5287F7A293}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A019F027-8123-4CDF-BE62-E60F7E5B0D6F}"/>
+    <workbookView xWindow="0" yWindow="636" windowWidth="17280" windowHeight="8964" xr2:uid="{A019F027-8123-4CDF-BE62-E60F7E5B0D6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>Confrence 100</t>
+  </si>
+  <si>
+    <t>Circle 98</t>
   </si>
 </sst>
 </file>
@@ -803,6 +809,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -819,9 +828,6 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -1138,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54BD848E-E297-4097-8BEE-9ABC561FDC7A}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.8" x14ac:dyDescent="0.3"/>
@@ -1157,20 +1163,20 @@
     <col min="15" max="18" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:14" ht="34.799999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F2" s="40" t="s">
+    <row r="1" spans="1:16" ht="23.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:16" ht="34.799999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41" t="s">
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="41"/>
-    </row>
-    <row r="3" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K2" s="42"/>
+    </row>
+    <row r="3" spans="1:16" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1204,7 +1210,7 @@
       </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
@@ -1238,11 +1244,11 @@
       <c r="K4" s="26">
         <v>80</v>
       </c>
-      <c r="L4" s="42" t="s">
+      <c r="L4" s="43" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>25</v>
       </c>
@@ -1276,9 +1282,9 @@
       <c r="K5" s="26">
         <v>100</v>
       </c>
-      <c r="L5" s="42"/>
-    </row>
-    <row r="6" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L5" s="43"/>
+    </row>
+    <row r="6" spans="1:16" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>35</v>
       </c>
@@ -1312,11 +1318,11 @@
       <c r="K6" s="21">
         <v>100</v>
       </c>
-      <c r="L6" s="43" t="s">
+      <c r="L6" s="44" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>41</v>
       </c>
@@ -1350,9 +1356,9 @@
       <c r="K7" s="31">
         <v>100</v>
       </c>
-      <c r="L7" s="44"/>
-    </row>
-    <row r="8" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L7" s="45"/>
+    </row>
+    <row r="8" spans="1:16" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>23</v>
       </c>
@@ -1386,11 +1392,11 @@
       <c r="K8" s="21">
         <v>100</v>
       </c>
-      <c r="L8" s="43" t="s">
+      <c r="L8" s="44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
       <c r="B9" s="38">
         <v>6</v>
@@ -1406,9 +1412,9 @@
       <c r="I9" s="24"/>
       <c r="J9" s="25"/>
       <c r="K9" s="26"/>
-      <c r="L9" s="45"/>
-    </row>
-    <row r="10" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L9" s="46"/>
+    </row>
+    <row r="10" spans="1:16" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>39</v>
       </c>
@@ -1442,15 +1448,21 @@
       <c r="K10" s="26">
         <v>90</v>
       </c>
-      <c r="L10" s="45"/>
+      <c r="L10" s="46"/>
       <c r="M10" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="N10" s="46" t="s">
+      <c r="N10" s="40" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O10" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="P10" s="40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>33</v>
       </c>
@@ -1484,9 +1496,9 @@
       <c r="K11" s="26">
         <v>95</v>
       </c>
-      <c r="L11" s="45"/>
-    </row>
-    <row r="12" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L11" s="46"/>
+    </row>
+    <row r="12" spans="1:16" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>31</v>
       </c>
@@ -1518,11 +1530,11 @@
         <v>105</v>
       </c>
       <c r="K12" s="31">
-        <v>110</v>
-      </c>
-      <c r="L12" s="44"/>
-    </row>
-    <row r="13" spans="1:14" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="L12" s="45"/>
+    </row>
+    <row r="13" spans="1:16" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>36</v>
       </c>
@@ -1552,7 +1564,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="23.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="23.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="1"/>
@@ -1565,7 +1577,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="39" t="s">
         <v>42</v>
@@ -1580,7 +1592,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>

</xml_diff>

<commit_message>
mohsen saeed abadi degree added
</commit_message>
<xml_diff>
--- a/Degree.xlsx
+++ b/Degree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\AP Tamrin 3 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0127A0C8-8EAC-4B1D-8AC6-BF5287F7A293}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58DEC02-BC9B-47F2-9543-CA69C054E2C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="636" windowWidth="17280" windowHeight="8964" xr2:uid="{A019F027-8123-4CDF-BE62-E60F7E5B0D6F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A019F027-8123-4CDF-BE62-E60F7E5B0D6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -171,12 +171,6 @@
     <t>90 90per</t>
   </si>
   <si>
-    <t>70per</t>
-  </si>
-  <si>
-    <t>90per</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Mokhtalet100</t>
   </si>
   <si>
@@ -187,6 +181,12 @@
   </si>
   <si>
     <t>Circle 98</t>
+  </si>
+  <si>
+    <t>68 70per</t>
+  </si>
+  <si>
+    <t>76.5 90per</t>
   </si>
 </sst>
 </file>
@@ -1146,8 +1146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54BD848E-E297-4097-8BEE-9ABC561FDC7A}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.8" x14ac:dyDescent="0.3"/>
@@ -1450,16 +1450,16 @@
       </c>
       <c r="L10" s="46"/>
       <c r="M10" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="P10" s="40" t="s">
         <v>49</v>
-      </c>
-      <c r="N10" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="O10" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="P10" s="40" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1550,15 +1550,23 @@
       <c r="E13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="34"/>
+      <c r="F13" s="32">
+        <v>93</v>
+      </c>
+      <c r="G13" s="33">
+        <v>100</v>
+      </c>
+      <c r="H13" s="33">
+        <v>100</v>
+      </c>
+      <c r="I13" s="34">
+        <v>100</v>
+      </c>
       <c r="J13" s="35" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="K13" s="36" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
safari degree added with so delay
</commit_message>
<xml_diff>
--- a/Degree.xlsx
+++ b/Degree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\AP Tamrin 3 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58DEC02-BC9B-47F2-9543-CA69C054E2C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FB3001-E9C8-4026-B2EF-B446B2C9B19C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A019F027-8123-4CDF-BE62-E60F7E5B0D6F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>76.5 90per</t>
+  </si>
+  <si>
+    <t>36.4 70per</t>
+  </si>
+  <si>
+    <t>45 90per</t>
   </si>
 </sst>
 </file>
@@ -694,7 +700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -828,6 +834,12 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -1147,7 +1159,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.8" x14ac:dyDescent="0.3"/>
@@ -1586,18 +1598,32 @@
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B15" s="2"/>
+      <c r="B15" s="47"/>
       <c r="C15" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+      <c r="D15" s="47">
+        <v>97412301</v>
+      </c>
+      <c r="E15" s="47"/>
+      <c r="F15" s="48">
+        <v>110</v>
+      </c>
+      <c r="G15" s="48">
+        <v>80</v>
+      </c>
+      <c r="H15" s="48">
+        <v>83</v>
+      </c>
+      <c r="I15" s="48">
+        <v>92</v>
+      </c>
+      <c r="J15" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="K15" s="48" t="s">
+        <v>52</v>
+      </c>
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
@@ -1605,12 +1631,12 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">

</xml_diff>